<commit_message>
Nuevos cambios excel pabot
</commit_message>
<xml_diff>
--- a/test/Datos_sinamope.xlsx
+++ b/test/Datos_sinamope.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
   <si>
     <t>DONOVAN GUTIERREZ</t>
   </si>
@@ -383,12 +383,12 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" customWidth="1"/>
     <col min="3" max="3" width="50.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -522,25 +522,190 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B8" s="2"/>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B9" s="2"/>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>8</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>

</xml_diff>